<commit_message>
committing uncommitted changes from September 2022
</commit_message>
<xml_diff>
--- a/covid-data/covid_deaths_manual_notes_wikipedia_pop.xlsx
+++ b/covid-data/covid_deaths_manual_notes_wikipedia_pop.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/urban_density_covid_linkage/covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{0371A38D-0207-49BE-8412-2B4E9A7EF0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01BCF6FC-BCE0-4E41-B62F-A8FFB3ED10DF}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:40009_{0371A38D-0207-49BE-8412-2B4E9A7EF0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E43F7E6-068B-490E-A22D-CFF76716F757}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1497,13 +1497,16 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J55" sqref="A1:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="9" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="7" width="21.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1550,7 +1553,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1725,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1736,7 +1739,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1865,7 +1868,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2544,7 +2547,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -2716,7 +2719,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -2888,7 +2891,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2931,7 +2934,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -3183,7 +3186,7 @@
         <v>44794</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -3379,9 +3382,7 @@
   </sheetData>
   <autoFilter ref="A1:L55" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="7">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>